<commit_message>
Added patient registry support
</commit_message>
<xml_diff>
--- a/vp_test_input/EJPRD_Resource_Metadata_template.xlsx
+++ b/vp_test_input/EJPRD_Resource_Metadata_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lumconline-my.sharepoint.com/personal/j_d_wijnbergen_lumc_nl/Documents/PhD/code/fdp_populator/vp_test_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{518A5C42-F99B-497C-83E2-4BAAA0FC4C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8D0D656-F62C-4DF7-AA96-831AB97A7772}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{518A5C42-F99B-497C-83E2-4BAAA0FC4C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87DA1501-8385-45F1-AD94-05BEDE6C893D}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2393" windowWidth="21600" windowHeight="12772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2393" windowWidth="21600" windowHeight="12772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organisation" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5767" uniqueCount="4758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5774" uniqueCount="4762">
   <si>
     <t>Title</t>
   </si>
@@ -14299,6 +14299,18 @@
   </si>
   <si>
     <t>http://example.org/Test_organisation; http://example.org/Test_organisation_parent_organisation</t>
+  </si>
+  <si>
+    <t>Test patient registry</t>
+  </si>
+  <si>
+    <t>Patient registry for testing reading of excel file and pushing RDF to a FDP</t>
+  </si>
+  <si>
+    <t>http://example.org/test_patient_registry; http://example.org/extra_information</t>
+  </si>
+  <si>
+    <t>Patient registry</t>
   </si>
 </sst>
 </file>
@@ -14700,8 +14712,8 @@
   </sheetPr>
   <dimension ref="A1:E994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -21706,8 +21718,8 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -21763,13 +21775,28 @@
         <v>4752</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="10"/>
+    <row r="3" spans="1:7" ht="89.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>4758</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>4759</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4754</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>4755</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>4747</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>4760</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>4761</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
@@ -29755,6 +29782,7 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{7F81CC35-14A2-41B8-AF73-5F84A58D3C48}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{BFD01080-8BDF-42F1-8365-23F730393057}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>